<commit_message>
ETL: ETL Project Finished
</commit_message>
<xml_diff>
--- a/Resources/Sheets/Cargos.xlsx
+++ b/Resources/Sheets/Cargos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0 - Personal\portfolio\projects\0\Resources\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113293EB-BF98-40C0-97A3-C5B26E7F7332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C20C9D-B1A0-43B3-B836-AE5944D9C730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{50626142-4B70-4B4D-91F0-E10C2AEFA775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28950" windowHeight="15480" xr2:uid="{50626142-4B70-4B4D-91F0-E10C2AEFA775}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -747,9 +747,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,7 +774,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -883,8 +885,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F0FDF5D-7AD2-4095-A396-9D96C56D85A5}" name="tCargos" displayName="tCargos" ref="A1:B240" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B240" xr:uid="{1F0FDF5D-7AD2-4095-A396-9D96C56D85A5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F9366710-8F8D-4AB5-AB1F-CD99CF3FBF27}" name="id_cargo" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{6CAE552E-2F4E-44A3-BC4C-71E5F29747AA}" name="Cargo" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F9366710-8F8D-4AB5-AB1F-CD99CF3FBF27}" name="id_cargo" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6CAE552E-2F4E-44A3-BC4C-71E5F29747AA}" name="Cargo" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1190,17 +1192,17 @@
   <dimension ref="A1:B240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="12" style="3" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1208,7 +1210,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1216,7 +1218,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1224,7 +1226,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1232,7 +1234,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1240,7 +1242,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1248,7 +1250,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1256,7 +1258,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1264,7 +1266,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1272,7 +1274,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1280,7 +1282,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1288,7 +1290,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>91</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1296,7 +1298,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>107</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1304,7 +1306,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>117</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1312,7 +1314,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>133</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1320,7 +1322,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1328,7 +1330,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>219</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1336,7 +1338,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>220</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1344,7 +1346,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>221</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1352,7 +1354,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>222</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1360,7 +1362,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>227</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1368,7 +1370,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>229</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1376,7 +1378,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>230</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1384,7 +1386,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>233</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1392,7 +1394,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>236</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1400,7 +1402,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>237</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1408,7 +1410,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>240</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1416,7 +1418,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>242</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1424,7 +1426,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>244</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1432,7 +1434,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>246</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1440,7 +1442,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>249</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1448,7 +1450,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>251</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1456,7 +1458,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>260</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1464,7 +1466,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>267</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1472,7 +1474,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>268</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1480,7 +1482,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>271</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1488,7 +1490,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>277</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1496,7 +1498,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>278</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1504,7 +1506,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>281</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1512,7 +1514,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>293</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1520,7 +1522,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>297</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1528,7 +1530,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>302</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1536,7 +1538,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>305</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1544,7 +1546,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>307</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1552,7 +1554,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>319</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1560,7 +1562,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>321</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1568,7 +1570,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>322</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1576,7 +1578,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>329</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1584,7 +1586,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>330</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1592,7 +1594,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>331</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1600,7 +1602,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>334</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1608,7 +1610,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>337</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1616,7 +1618,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>338</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1624,7 +1626,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>340</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1632,7 +1634,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>341</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1640,7 +1642,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>343</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1648,7 +1650,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>346</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1656,7 +1658,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>347</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1664,7 +1666,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>349</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1672,7 +1674,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>352</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1680,7 +1682,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>354</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1688,7 +1690,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>355</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1696,7 +1698,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>357</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1704,7 +1706,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>359</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1712,7 +1714,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>360</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1720,7 +1722,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>362</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1728,7 +1730,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>366</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1736,7 +1738,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>367</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1744,7 +1746,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>368</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1752,7 +1754,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>370</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1760,7 +1762,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>371</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -1768,7 +1770,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>373</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1776,7 +1778,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>374</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1784,7 +1786,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>375</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -1792,7 +1794,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>376</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -1800,7 +1802,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>378</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1808,7 +1810,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>379</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1816,7 +1818,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>380</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1824,7 +1826,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>381</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1832,7 +1834,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>382</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -1840,7 +1842,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>383</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -1848,7 +1850,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>385</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -1856,7 +1858,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>387</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -1864,7 +1866,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>388</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -1872,7 +1874,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>389</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -1880,7 +1882,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>393</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -1888,7 +1890,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>394</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -1896,7 +1898,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>396</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -1904,7 +1906,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>397</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -1912,7 +1914,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>398</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -1920,7 +1922,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>402</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -1928,7 +1930,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>406</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -1936,7 +1938,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>407</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -1944,7 +1946,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>411</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -1952,7 +1954,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>414</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -1960,7 +1962,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>416</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -1968,7 +1970,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>417</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -1976,7 +1978,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>419</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -1984,7 +1986,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>420</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -1992,7 +1994,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>422</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2000,7 +2002,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>423</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -2008,7 +2010,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="A102" s="2">
         <v>425</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -2016,7 +2018,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103" s="2">
         <v>426</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -2024,7 +2026,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+      <c r="A104" s="2">
         <v>427</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -2032,7 +2034,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="A105" s="2">
         <v>430</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -2040,7 +2042,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+      <c r="A106" s="2">
         <v>431</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -2048,7 +2050,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="A107" s="2">
         <v>432</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -2056,7 +2058,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="A108" s="2">
         <v>434</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -2064,7 +2066,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="A109" s="2">
         <v>440</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -2072,7 +2074,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="A110" s="2">
         <v>444</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -2080,7 +2082,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="A111" s="2">
         <v>446</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -2088,7 +2090,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+      <c r="A112" s="2">
         <v>448</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -2096,7 +2098,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="A113" s="2">
         <v>449</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -2104,7 +2106,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+      <c r="A114" s="2">
         <v>451</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -2112,7 +2114,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115" s="2">
         <v>455</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -2120,7 +2122,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+      <c r="A116" s="2">
         <v>456</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -2128,7 +2130,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+      <c r="A117" s="2">
         <v>457</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -2136,7 +2138,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+      <c r="A118" s="2">
         <v>488</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -2144,7 +2146,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+      <c r="A119" s="2">
         <v>496</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -2152,7 +2154,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+      <c r="A120" s="2">
         <v>507</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -2160,7 +2162,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+      <c r="A121" s="2">
         <v>514</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -2168,7 +2170,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+      <c r="A122" s="2">
         <v>1001</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -2176,7 +2178,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+      <c r="A123" s="2">
         <v>1002</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -2184,7 +2186,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+      <c r="A124" s="2">
         <v>2001</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -2192,7 +2194,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+      <c r="A125" s="2">
         <v>2003</v>
       </c>
       <c r="B125" s="1" t="s">
@@ -2200,7 +2202,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+      <c r="A126" s="2">
         <v>3003</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -2208,7 +2210,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+      <c r="A127" s="2">
         <v>3004</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -2216,7 +2218,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+      <c r="A128" s="2">
         <v>4002</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -2224,7 +2226,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+      <c r="A129" s="2">
         <v>6004</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -2232,7 +2234,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+      <c r="A130" s="2">
         <v>7003</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -2240,7 +2242,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+      <c r="A131" s="2">
         <v>8002</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -2248,7 +2250,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
+      <c r="A132" s="2">
         <v>9001</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -2256,7 +2258,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+      <c r="A133" s="2">
         <v>10002</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -2264,7 +2266,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
+      <c r="A134" s="2">
         <v>11001</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -2272,7 +2274,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
+      <c r="A135" s="2">
         <v>12001</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -2280,7 +2282,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
+      <c r="A136" s="2">
         <v>14001</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -2288,7 +2290,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+      <c r="A137" s="2">
         <v>14002</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -2296,7 +2298,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+      <c r="A138" s="2">
         <v>14003</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -2304,7 +2306,7 @@
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+      <c r="A139" s="2">
         <v>17001</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -2312,7 +2314,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+      <c r="A140" s="2">
         <v>17002</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -2320,7 +2322,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
+      <c r="A141" s="2">
         <v>17003</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -2328,7 +2330,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+      <c r="A142" s="2">
         <v>18001</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -2336,7 +2338,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+      <c r="A143" s="2">
         <v>20001</v>
       </c>
       <c r="B143" s="1" t="s">
@@ -2344,7 +2346,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+      <c r="A144" s="2">
         <v>20002</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -2352,7 +2354,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+      <c r="A145" s="2">
         <v>24001</v>
       </c>
       <c r="B145" s="1" t="s">
@@ -2360,7 +2362,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+      <c r="A146" s="2">
         <v>24002</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -2368,7 +2370,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+      <c r="A147" s="2">
         <v>25001</v>
       </c>
       <c r="B147" s="1" t="s">
@@ -2376,7 +2378,7 @@
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
+      <c r="A148" s="2">
         <v>26003</v>
       </c>
       <c r="B148" s="1" t="s">
@@ -2384,7 +2386,7 @@
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
+      <c r="A149" s="2">
         <v>27001</v>
       </c>
       <c r="B149" s="1" t="s">
@@ -2392,7 +2394,7 @@
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+      <c r="A150" s="2">
         <v>29001</v>
       </c>
       <c r="B150" s="1" t="s">
@@ -2400,7 +2402,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+      <c r="A151" s="2">
         <v>32001</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -2408,7 +2410,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+      <c r="A152" s="2">
         <v>33001</v>
       </c>
       <c r="B152" s="1" t="s">
@@ -2416,7 +2418,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
+      <c r="A153" s="2">
         <v>35002</v>
       </c>
       <c r="B153" s="1" t="s">
@@ -2424,7 +2426,7 @@
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
+      <c r="A154" s="2">
         <v>35003</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -2432,7 +2434,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+      <c r="A155" s="2">
         <v>35004</v>
       </c>
       <c r="B155" s="1" t="s">
@@ -2440,7 +2442,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
+      <c r="A156" s="2">
         <v>36003</v>
       </c>
       <c r="B156" s="1" t="s">
@@ -2448,7 +2450,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+      <c r="A157" s="2">
         <v>37001</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -2456,7 +2458,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+      <c r="A158" s="2">
         <v>38002</v>
       </c>
       <c r="B158" s="1" t="s">
@@ -2464,7 +2466,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+      <c r="A159" s="2">
         <v>39001</v>
       </c>
       <c r="B159" s="1" t="s">
@@ -2472,7 +2474,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
+      <c r="A160" s="2">
         <v>40001</v>
       </c>
       <c r="B160" s="1" t="s">
@@ -2480,7 +2482,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+      <c r="A161" s="2">
         <v>41002</v>
       </c>
       <c r="B161" s="1" t="s">
@@ -2488,7 +2490,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+      <c r="A162" s="2">
         <v>42003</v>
       </c>
       <c r="B162" s="1" t="s">
@@ -2496,7 +2498,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+      <c r="A163" s="2">
         <v>43004</v>
       </c>
       <c r="B163" s="1" t="s">
@@ -2504,7 +2506,7 @@
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+      <c r="A164" s="2">
         <v>44001</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -2512,7 +2514,7 @@
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+      <c r="A165" s="2">
         <v>44002</v>
       </c>
       <c r="B165" s="1" t="s">
@@ -2520,7 +2522,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+      <c r="A166" s="2">
         <v>45001</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -2528,7 +2530,7 @@
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
+      <c r="A167" s="2">
         <v>46001</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -2536,7 +2538,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
+      <c r="A168" s="2">
         <v>48003</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -2544,7 +2546,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+      <c r="A169" s="2">
         <v>49001</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -2552,7 +2554,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
+      <c r="A170" s="2">
         <v>50001</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -2560,7 +2562,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+      <c r="A171" s="2">
         <v>51001</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -2568,7 +2570,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
+      <c r="A172" s="2">
         <v>52001</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -2576,7 +2578,7 @@
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+      <c r="A173" s="2">
         <v>53001</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -2584,7 +2586,7 @@
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+      <c r="A174" s="2">
         <v>54001</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -2592,7 +2594,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+      <c r="A175" s="2">
         <v>55001</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -2600,7 +2602,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
+      <c r="A176" s="2">
         <v>56001</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -2608,7 +2610,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
+      <c r="A177" s="2">
         <v>58001</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -2616,7 +2618,7 @@
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+      <c r="A178" s="2">
         <v>59001</v>
       </c>
       <c r="B178" s="1" t="s">
@@ -2624,7 +2626,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
+      <c r="A179" s="2">
         <v>60001</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -2632,7 +2634,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+      <c r="A180" s="2">
         <v>61001</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -2640,7 +2642,7 @@
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+      <c r="A181" s="2">
         <v>61004</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -2648,7 +2650,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+      <c r="A182" s="2">
         <v>62001</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -2656,7 +2658,7 @@
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+      <c r="A183" s="2">
         <v>63001</v>
       </c>
       <c r="B183" s="1" t="s">
@@ -2664,7 +2666,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+      <c r="A184" s="2">
         <v>63002</v>
       </c>
       <c r="B184" s="1" t="s">
@@ -2672,7 +2674,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
+      <c r="A185" s="2">
         <v>63003</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -2680,7 +2682,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
+      <c r="A186" s="2">
         <v>64004</v>
       </c>
       <c r="B186" s="1" t="s">
@@ -2688,7 +2690,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+      <c r="A187" s="2">
         <v>66001</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -2696,7 +2698,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+      <c r="A188" s="2">
         <v>69001</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -2704,7 +2706,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+      <c r="A189" s="2">
         <v>70001</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -2712,7 +2714,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
+      <c r="A190" s="2">
         <v>71001</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -2720,7 +2722,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+      <c r="A191" s="2">
         <v>72001</v>
       </c>
       <c r="B191" s="1" t="s">
@@ -2728,7 +2730,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+      <c r="A192" s="2">
         <v>75003</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -2736,7 +2738,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
+      <c r="A193" s="2">
         <v>74002</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -2744,7 +2746,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+      <c r="A194" s="2">
         <v>75002</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -2752,7 +2754,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
+      <c r="A195" s="2">
         <v>80001</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -2760,7 +2762,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
+      <c r="A196" s="2">
         <v>81001</v>
       </c>
       <c r="B196" s="1" t="s">
@@ -2768,7 +2770,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
+      <c r="A197" s="2">
         <v>82001</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -2776,7 +2778,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+      <c r="A198" s="2">
         <v>83004</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -2784,7 +2786,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+      <c r="A199" s="2">
         <v>83006</v>
       </c>
       <c r="B199" s="1" t="s">
@@ -2792,7 +2794,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
+      <c r="A200" s="2">
         <v>84001</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -2800,7 +2802,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
+      <c r="A201" s="2">
         <v>85001</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -2808,7 +2810,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
+      <c r="A202" s="2">
         <v>87001</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -2816,7 +2818,7 @@
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
+      <c r="A203" s="2">
         <v>88001</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -2824,7 +2826,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
+      <c r="A204" s="2">
         <v>89001</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -2832,7 +2834,7 @@
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
+      <c r="A205" s="2">
         <v>90002</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -2840,7 +2842,7 @@
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
+      <c r="A206" s="2">
         <v>93002</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -2848,7 +2850,7 @@
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
+      <c r="A207" s="2">
         <v>94001</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -2856,7 +2858,7 @@
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
+      <c r="A208" s="2">
         <v>94002</v>
       </c>
       <c r="B208" s="1" t="s">
@@ -2864,7 +2866,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
+      <c r="A209" s="2">
         <v>95001</v>
       </c>
       <c r="B209" s="1" t="s">
@@ -2872,7 +2874,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
+      <c r="A210" s="2">
         <v>96002</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -2880,7 +2882,7 @@
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+      <c r="A211" s="2">
         <v>98001</v>
       </c>
       <c r="B211" s="1" t="s">
@@ -2888,7 +2890,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
+      <c r="A212" s="2">
         <v>99001</v>
       </c>
       <c r="B212" s="1" t="s">
@@ -2896,7 +2898,7 @@
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
+      <c r="A213" s="2">
         <v>100001</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -2904,7 +2906,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="1">
+      <c r="A214" s="2">
         <v>101001</v>
       </c>
       <c r="B214" s="1" t="s">
@@ -2912,7 +2914,7 @@
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+      <c r="A215" s="2">
         <v>102001</v>
       </c>
       <c r="B215" s="1" t="s">
@@ -2920,7 +2922,7 @@
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="A216" s="2">
         <v>102003</v>
       </c>
       <c r="B216" s="1" t="s">
@@ -2928,7 +2930,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
+      <c r="A217" s="2">
         <v>109001</v>
       </c>
       <c r="B217" s="1" t="s">
@@ -2936,7 +2938,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
+      <c r="A218" s="2">
         <v>110001</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -2944,7 +2946,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+      <c r="A219" s="2">
         <v>112001</v>
       </c>
       <c r="B219" s="1" t="s">
@@ -2952,7 +2954,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="1">
+      <c r="A220" s="2">
         <v>113001</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -2960,7 +2962,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="1">
+      <c r="A221" s="2">
         <v>114001</v>
       </c>
       <c r="B221" s="1" t="s">
@@ -2968,7 +2970,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="1">
+      <c r="A222" s="2">
         <v>118001</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -2976,7 +2978,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
+      <c r="A223" s="2">
         <v>119001</v>
       </c>
       <c r="B223" s="1" t="s">
@@ -2984,7 +2986,7 @@
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+      <c r="A224" s="2">
         <v>120001</v>
       </c>
       <c r="B224" s="1" t="s">
@@ -2992,7 +2994,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
+      <c r="A225" s="2">
         <v>123001</v>
       </c>
       <c r="B225" s="1" t="s">
@@ -3000,7 +3002,7 @@
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="1">
+      <c r="A226" s="2">
         <v>125001</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -3008,7 +3010,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
+      <c r="A227" s="2">
         <v>126001</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -3016,7 +3018,7 @@
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+      <c r="A228" s="2">
         <v>127001</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -3024,7 +3026,7 @@
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
+      <c r="A229" s="2">
         <v>129001</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -3032,7 +3034,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
+      <c r="A230" s="2">
         <v>130001</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -3040,7 +3042,7 @@
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="1">
+      <c r="A231" s="2">
         <v>131001</v>
       </c>
       <c r="B231" s="1" t="s">
@@ -3048,7 +3050,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
+      <c r="A232" s="2">
         <v>132001</v>
       </c>
       <c r="B232" s="1" t="s">
@@ -3056,7 +3058,7 @@
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
+      <c r="A233" s="2">
         <v>134001</v>
       </c>
       <c r="B233" s="1" t="s">
@@ -3064,7 +3066,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
+      <c r="A234" s="2">
         <v>135001</v>
       </c>
       <c r="B234" s="1" t="s">
@@ -3072,7 +3074,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="1">
+      <c r="A235" s="2">
         <v>136001</v>
       </c>
       <c r="B235" s="1" t="s">
@@ -3080,7 +3082,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="1">
+      <c r="A236" s="2">
         <v>139001</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -3088,7 +3090,7 @@
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
+      <c r="A237" s="2">
         <v>140001</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -3096,7 +3098,7 @@
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="1">
+      <c r="A238" s="2">
         <v>141001</v>
       </c>
       <c r="B238" s="1" t="s">
@@ -3104,7 +3106,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
+      <c r="A239" s="2">
         <v>142001</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -3112,7 +3114,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
+      <c r="A240" s="2">
         <v>144001</v>
       </c>
       <c r="B240" s="1" t="s">

</xml_diff>